<commit_message>
-updated xlsx -safe fail for battery
</commit_message>
<xml_diff>
--- a/inst/extdata/China_ Blast Furnace Starting Rate (247)_ Nationwide.xlsx
+++ b/inst/extdata/China_ Blast Furnace Starting Rate (247)_ Nationwide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobol\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\CREA-China\monthly snapshot\wind data templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290A43F3-CF08-4577-B416-BA404D2C3164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A240E09-F980-4034-94A4-C1AC458346D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="19245" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="China_ Blast Furnace Starting R" sheetId="1" r:id="rId1"/>
@@ -95,16 +95,16 @@
     <t>Source</t>
   </si>
   <si>
-    <t>According to the Press Finishing</t>
-  </si>
-  <si>
     <t>Update</t>
   </si>
   <si>
-    <t>2018-03-02:2023-07-07</t>
+    <t>2018-03-02:2023-11-10</t>
   </si>
   <si>
-    <t>2023-07-07</t>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>2023-11-10</t>
   </si>
 </sst>
 </file>
@@ -505,19 +505,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C284"/>
+  <dimension ref="A1:C302"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="str">
         <f>[1]!edb()</f>
-        <v>Wind</v>
+        <v>error!</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -569,10 +570,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -580,15 +581,15 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>15</v>
@@ -602,10 +603,10 @@
         <v>43161</v>
       </c>
       <c r="B9" s="2">
-        <v>75.489999999999995</v>
+        <v>75.47</v>
       </c>
       <c r="C9" s="2">
-        <v>74.58</v>
+        <v>74.56</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -613,10 +614,10 @@
         <v>43168</v>
       </c>
       <c r="B10" s="2">
-        <v>75.150000000000006</v>
+        <v>75.13</v>
       </c>
       <c r="C10" s="2">
-        <v>74.95</v>
+        <v>74.97</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -624,10 +625,10 @@
         <v>43175</v>
       </c>
       <c r="B11" s="2">
-        <v>75.260000000000005</v>
+        <v>75.27</v>
       </c>
       <c r="C11" s="2">
-        <v>74.53</v>
+        <v>74.510000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -635,10 +636,10 @@
         <v>43182</v>
       </c>
       <c r="B12" s="2">
-        <v>76.31</v>
+        <v>76.33</v>
       </c>
       <c r="C12" s="2">
-        <v>74.86</v>
+        <v>74.88</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -646,10 +647,10 @@
         <v>43189</v>
       </c>
       <c r="B13" s="2">
-        <v>77.930000000000007</v>
+        <v>77.95</v>
       </c>
       <c r="C13" s="2">
-        <v>75.75</v>
+        <v>75.77</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -657,10 +658,10 @@
         <v>43199</v>
       </c>
       <c r="B14" s="2">
-        <v>78.510000000000005</v>
+        <v>78.53</v>
       </c>
       <c r="C14" s="2">
-        <v>76.78</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -668,10 +669,10 @@
         <v>43203</v>
       </c>
       <c r="B15" s="2">
-        <v>79.67</v>
+        <v>79.69</v>
       </c>
       <c r="C15" s="2">
-        <v>77.92</v>
+        <v>77.94</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -679,10 +680,10 @@
         <v>43210</v>
       </c>
       <c r="B16" s="2">
-        <v>78.86</v>
+        <v>78.84</v>
       </c>
       <c r="C16" s="2">
-        <v>78.25</v>
+        <v>78.27</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -690,10 +691,10 @@
         <v>43217</v>
       </c>
       <c r="B17" s="2">
-        <v>78.510000000000005</v>
+        <v>78.489999999999995</v>
       </c>
       <c r="C17" s="2">
-        <v>77.400000000000006</v>
+        <v>77.38</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -701,10 +702,10 @@
         <v>43224</v>
       </c>
       <c r="B18" s="2">
-        <v>79.33</v>
+        <v>79.349999999999994</v>
       </c>
       <c r="C18" s="2">
-        <v>77.790000000000006</v>
+        <v>77.81</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -712,10 +713,10 @@
         <v>43231</v>
       </c>
       <c r="B19" s="2">
-        <v>80.489999999999995</v>
+        <v>80.510000000000005</v>
       </c>
       <c r="C19" s="2">
-        <v>79.12</v>
+        <v>79.14</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -723,10 +724,10 @@
         <v>43238</v>
       </c>
       <c r="B20" s="2">
-        <v>81.53</v>
+        <v>81.55</v>
       </c>
       <c r="C20" s="2">
-        <v>80.400000000000006</v>
+        <v>80.42</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -734,10 +735,10 @@
         <v>43245</v>
       </c>
       <c r="B21" s="2">
-        <v>83.39</v>
+        <v>83.41</v>
       </c>
       <c r="C21" s="2">
-        <v>81.489999999999995</v>
+        <v>81.510000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -745,10 +746,10 @@
         <v>43252</v>
       </c>
       <c r="B22" s="2">
-        <v>83.62</v>
+        <v>83.63</v>
       </c>
       <c r="C22" s="2">
-        <v>81.63</v>
+        <v>81.64</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -756,7 +757,7 @@
         <v>43259</v>
       </c>
       <c r="B23" s="2">
-        <v>83.28</v>
+        <v>83.26</v>
       </c>
       <c r="C23" s="2">
         <v>81.61</v>
@@ -767,10 +768,10 @@
         <v>43266</v>
       </c>
       <c r="B24" s="2">
-        <v>83.28</v>
+        <v>83.26</v>
       </c>
       <c r="C24" s="2">
-        <v>81.319999999999993</v>
+        <v>81.31</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -778,7 +779,7 @@
         <v>43273</v>
       </c>
       <c r="B25" s="2">
-        <v>83.16</v>
+        <v>83.15</v>
       </c>
       <c r="C25" s="2">
         <v>81.290000000000006</v>
@@ -789,10 +790,10 @@
         <v>43280</v>
       </c>
       <c r="B26" s="2">
-        <v>82.58</v>
+        <v>82.56</v>
       </c>
       <c r="C26" s="2">
-        <v>81.099999999999994</v>
+        <v>81.09</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -800,10 +801,10 @@
         <v>43287</v>
       </c>
       <c r="B27" s="2">
-        <v>83.28</v>
+        <v>83.3</v>
       </c>
       <c r="C27" s="2">
-        <v>81.430000000000007</v>
+        <v>81.45</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -811,7 +812,7 @@
         <v>43294</v>
       </c>
       <c r="B28" s="2">
-        <v>82.93</v>
+        <v>82.91</v>
       </c>
       <c r="C28" s="2">
         <v>81.52</v>
@@ -822,10 +823,10 @@
         <v>43301</v>
       </c>
       <c r="B29" s="2">
-        <v>83.16</v>
+        <v>83.17</v>
       </c>
       <c r="C29" s="2">
-        <v>81.66</v>
+        <v>81.67</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -833,10 +834,10 @@
         <v>43308</v>
       </c>
       <c r="B30" s="2">
-        <v>80.02</v>
+        <v>80</v>
       </c>
       <c r="C30" s="2">
-        <v>80</v>
+        <v>79.98</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -844,10 +845,10 @@
         <v>43315</v>
       </c>
       <c r="B31" s="2">
-        <v>79.44</v>
+        <v>79.42</v>
       </c>
       <c r="C31" s="2">
-        <v>79.69</v>
+        <v>79.67</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -855,10 +856,10 @@
         <v>43322</v>
       </c>
       <c r="B32" s="2">
-        <v>78.75</v>
+        <v>78.73</v>
       </c>
       <c r="C32" s="2">
-        <v>79.12</v>
+        <v>79.099999999999994</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -866,7 +867,7 @@
         <v>43329</v>
       </c>
       <c r="B33" s="2">
-        <v>78.75</v>
+        <v>78.73</v>
       </c>
       <c r="C33" s="2">
         <v>79.16</v>
@@ -877,7 +878,7 @@
         <v>43336</v>
       </c>
       <c r="B34" s="2">
-        <v>78.86</v>
+        <v>78.87</v>
       </c>
       <c r="C34" s="2">
         <v>79.239999999999995</v>
@@ -888,7 +889,7 @@
         <v>43343</v>
       </c>
       <c r="B35" s="2">
-        <v>79.09</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="C35" s="2">
         <v>79.25</v>
@@ -899,10 +900,10 @@
         <v>43350</v>
       </c>
       <c r="B36" s="2">
-        <v>79.44</v>
+        <v>79.459999999999994</v>
       </c>
       <c r="C36" s="2">
-        <v>79.61</v>
+        <v>79.63</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -910,10 +911,10 @@
         <v>43357</v>
       </c>
       <c r="B37" s="2">
-        <v>80.599999999999994</v>
+        <v>80.62</v>
       </c>
       <c r="C37" s="2">
-        <v>79.83</v>
+        <v>79.84</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -921,10 +922,10 @@
         <v>43364</v>
       </c>
       <c r="B38" s="2">
-        <v>80.489999999999995</v>
+        <v>80.48</v>
       </c>
       <c r="C38" s="2">
-        <v>80.430000000000007</v>
+        <v>80.45</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -932,10 +933,10 @@
         <v>43371</v>
       </c>
       <c r="B39" s="2">
-        <v>80.84</v>
+        <v>80.86</v>
       </c>
       <c r="C39" s="2">
-        <v>81.42</v>
+        <v>81.47</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -943,10 +944,10 @@
         <v>43378</v>
       </c>
       <c r="B40" s="2">
-        <v>80.02</v>
+        <v>80</v>
       </c>
       <c r="C40" s="2">
-        <v>81.61</v>
+        <v>81.62</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -954,10 +955,10 @@
         <v>43385</v>
       </c>
       <c r="B41" s="2">
-        <v>80.84</v>
+        <v>80.86</v>
       </c>
       <c r="C41" s="2">
-        <v>81.93</v>
+        <v>81.95</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -965,10 +966,10 @@
         <v>43392</v>
       </c>
       <c r="B42" s="2">
-        <v>80.37</v>
+        <v>80.349999999999994</v>
       </c>
       <c r="C42" s="2">
-        <v>82.04</v>
+        <v>82.05</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -976,10 +977,10 @@
         <v>43399</v>
       </c>
       <c r="B43" s="2">
-        <v>80.14</v>
+        <v>80.13</v>
       </c>
       <c r="C43" s="2">
-        <v>81.66</v>
+        <v>81.64</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -987,7 +988,7 @@
         <v>43406</v>
       </c>
       <c r="B44" s="2">
-        <v>79.44</v>
+        <v>79.42</v>
       </c>
       <c r="C44" s="2">
         <v>81.709999999999994</v>
@@ -998,10 +999,10 @@
         <v>43413</v>
       </c>
       <c r="B45" s="2">
-        <v>79.09</v>
+        <v>79.069999999999993</v>
       </c>
       <c r="C45" s="2">
-        <v>80.75</v>
+        <v>80.73</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1009,10 +1010,10 @@
         <v>43420</v>
       </c>
       <c r="B46" s="2">
-        <v>78.400000000000006</v>
+        <v>78.37</v>
       </c>
       <c r="C46" s="2">
-        <v>80.5</v>
+        <v>80.489999999999995</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1020,10 +1021,10 @@
         <v>43427</v>
       </c>
       <c r="B47" s="2">
-        <v>77.58</v>
+        <v>77.56</v>
       </c>
       <c r="C47" s="2">
-        <v>79.23</v>
+        <v>79.209999999999994</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1031,7 +1032,7 @@
         <v>43434</v>
       </c>
       <c r="B48" s="2">
-        <v>76.89</v>
+        <v>76.87</v>
       </c>
       <c r="C48" s="2">
         <v>79.31</v>
@@ -1042,10 +1043,10 @@
         <v>43441</v>
       </c>
       <c r="B49" s="2">
-        <v>76.31</v>
+        <v>76.290000000000006</v>
       </c>
       <c r="C49" s="2">
-        <v>78.81</v>
+        <v>78.790000000000006</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1053,10 +1054,10 @@
         <v>43448</v>
       </c>
       <c r="B50" s="2">
-        <v>76.19</v>
+        <v>76.180000000000007</v>
       </c>
       <c r="C50" s="2">
-        <v>78.13</v>
+        <v>78.11</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1064,10 +1065,10 @@
         <v>43455</v>
       </c>
       <c r="B51" s="2">
-        <v>75.260000000000005</v>
+        <v>75.239999999999995</v>
       </c>
       <c r="C51" s="2">
-        <v>77.790000000000006</v>
+        <v>77.77</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1075,10 +1076,10 @@
         <v>43462</v>
       </c>
       <c r="B52" s="2">
-        <v>75.489999999999995</v>
+        <v>75.5</v>
       </c>
       <c r="C52" s="2">
-        <v>76.8</v>
+        <v>76.78</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1086,10 +1087,10 @@
         <v>43469</v>
       </c>
       <c r="B53" s="2">
-        <v>74.8</v>
+        <v>74.78</v>
       </c>
       <c r="C53" s="2">
-        <v>76.03</v>
+        <v>76.010000000000005</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1097,10 +1098,10 @@
         <v>43476</v>
       </c>
       <c r="B54" s="2">
-        <v>75.03</v>
+        <v>75.040000000000006</v>
       </c>
       <c r="C54" s="2">
-        <v>76.42</v>
+        <v>76.44</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1108,7 +1109,7 @@
         <v>43483</v>
       </c>
       <c r="B55" s="2">
-        <v>75.84</v>
+        <v>75.88</v>
       </c>
       <c r="C55" s="2">
         <v>76.45</v>
@@ -1119,10 +1120,10 @@
         <v>43490</v>
       </c>
       <c r="B56" s="2">
-        <v>77.12</v>
+        <v>77.14</v>
       </c>
       <c r="C56" s="2">
-        <v>77.239999999999995</v>
+        <v>77.260000000000005</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1130,10 +1131,10 @@
         <v>43497</v>
       </c>
       <c r="B57" s="2">
-        <v>77.58</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="C57" s="2">
-        <v>77.790000000000006</v>
+        <v>77.81</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1141,10 +1142,10 @@
         <v>43507</v>
       </c>
       <c r="B58" s="2">
-        <v>77.239999999999995</v>
+        <v>77.22</v>
       </c>
       <c r="C58" s="2">
-        <v>77.989999999999995</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1152,7 +1153,7 @@
         <v>43511</v>
       </c>
       <c r="B59" s="2">
-        <v>77.239999999999995</v>
+        <v>77.22</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
@@ -1163,10 +1164,10 @@
         <v>43518</v>
       </c>
       <c r="B60" s="2">
-        <v>77.58</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="C60" s="2">
-        <v>79.06</v>
+        <v>79.08</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1174,10 +1175,10 @@
         <v>43525</v>
       </c>
       <c r="B61" s="2">
-        <v>77.239999999999995</v>
+        <v>77.22</v>
       </c>
       <c r="C61" s="2">
-        <v>78.88</v>
+        <v>78.87</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1185,10 +1186,10 @@
         <v>43532</v>
       </c>
       <c r="B62" s="2">
-        <v>74.099999999999994</v>
+        <v>73.94</v>
       </c>
       <c r="C62" s="2">
-        <v>76.959999999999994</v>
+        <v>76.86</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1196,10 +1197,10 @@
         <v>43539</v>
       </c>
       <c r="B63" s="2">
-        <v>73.87</v>
+        <v>73.86</v>
       </c>
       <c r="C63" s="2">
-        <v>76.58</v>
+        <v>76.56</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1207,10 +1208,10 @@
         <v>43546</v>
       </c>
       <c r="B64" s="2">
-        <v>75.03</v>
+        <v>75.05</v>
       </c>
       <c r="C64" s="2">
-        <v>77.5</v>
+        <v>77.52</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1218,10 +1219,10 @@
         <v>43553</v>
       </c>
       <c r="B65" s="2">
-        <v>75.73</v>
+        <v>75.75</v>
       </c>
       <c r="C65" s="2">
-        <v>78.31</v>
+        <v>78.33</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1229,10 +1230,10 @@
         <v>43559</v>
       </c>
       <c r="B66" s="2">
-        <v>79.91</v>
+        <v>79.930000000000007</v>
       </c>
       <c r="C66" s="2">
-        <v>79.45</v>
+        <v>79.47</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1240,10 +1241,10 @@
         <v>43567</v>
       </c>
       <c r="B67" s="2">
-        <v>81.42</v>
+        <v>81.44</v>
       </c>
       <c r="C67" s="2">
-        <v>81.739999999999995</v>
+        <v>81.760000000000005</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1251,10 +1252,10 @@
         <v>43574</v>
       </c>
       <c r="B68" s="2">
-        <v>82.46</v>
+        <v>82.48</v>
       </c>
       <c r="C68" s="2">
-        <v>83.05</v>
+        <v>83.07</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1262,10 +1263,10 @@
         <v>43581</v>
       </c>
       <c r="B69" s="2">
-        <v>83.16</v>
+        <v>83.18</v>
       </c>
       <c r="C69" s="2">
-        <v>83.54</v>
+        <v>83.56</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1273,10 +1274,10 @@
         <v>43590</v>
       </c>
       <c r="B70" s="2">
-        <v>83.39</v>
+        <v>83.4</v>
       </c>
       <c r="C70" s="2">
-        <v>83.96</v>
+        <v>83.98</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1284,10 +1285,10 @@
         <v>43595</v>
       </c>
       <c r="B71" s="2">
-        <v>81.88</v>
+        <v>81.8</v>
       </c>
       <c r="C71" s="2">
-        <v>83.43</v>
+        <v>83.41</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1295,10 +1296,10 @@
         <v>43602</v>
       </c>
       <c r="B72" s="2">
-        <v>82.23</v>
+        <v>82.25</v>
       </c>
       <c r="C72" s="2">
-        <v>83.69</v>
+        <v>83.7</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1306,10 +1307,10 @@
         <v>43609</v>
       </c>
       <c r="B73" s="2">
-        <v>84.32</v>
+        <v>84.34</v>
       </c>
       <c r="C73" s="2">
-        <v>84.17</v>
+        <v>84.19</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1317,10 +1318,10 @@
         <v>43616</v>
       </c>
       <c r="B74" s="2">
-        <v>84.67</v>
+        <v>84.69</v>
       </c>
       <c r="C74" s="2">
-        <v>84.37</v>
+        <v>84.38</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1328,10 +1329,10 @@
         <v>43622</v>
       </c>
       <c r="B75" s="2">
-        <v>84.9</v>
+        <v>84.91</v>
       </c>
       <c r="C75" s="2">
-        <v>85.05</v>
+        <v>85.07</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1339,7 +1340,7 @@
         <v>43630</v>
       </c>
       <c r="B76" s="2">
-        <v>84.67</v>
+        <v>84.66</v>
       </c>
       <c r="C76" s="2">
         <v>85.03</v>
@@ -1350,10 +1351,10 @@
         <v>43637</v>
       </c>
       <c r="B77" s="2">
-        <v>84.44</v>
+        <v>84.43</v>
       </c>
       <c r="C77" s="2">
-        <v>84.54</v>
+        <v>84.52</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1361,10 +1362,10 @@
         <v>43644</v>
       </c>
       <c r="B78" s="2">
-        <v>81.650000000000006</v>
+        <v>81.63</v>
       </c>
       <c r="C78" s="2">
-        <v>83.81</v>
+        <v>83.79</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1372,10 +1373,10 @@
         <v>43651</v>
       </c>
       <c r="B79" s="2">
-        <v>80.14</v>
+        <v>80.12</v>
       </c>
       <c r="C79" s="2">
-        <v>81.13</v>
+        <v>81.11</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1383,10 +1384,10 @@
         <v>43658</v>
       </c>
       <c r="B80" s="2">
-        <v>79.91</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="C80" s="2">
-        <v>80.849999999999994</v>
+        <v>80.84</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1394,10 +1395,10 @@
         <v>43665</v>
       </c>
       <c r="B81" s="2">
-        <v>80.37</v>
+        <v>80.39</v>
       </c>
       <c r="C81" s="2">
-        <v>80.430000000000007</v>
+        <v>80.41</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1405,10 +1406,10 @@
         <v>43672</v>
       </c>
       <c r="B82" s="2">
-        <v>80.14</v>
+        <v>80.13</v>
       </c>
       <c r="C82" s="2">
-        <v>80.73</v>
+        <v>80.75</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1416,10 +1417,10 @@
         <v>43679</v>
       </c>
       <c r="B83" s="2">
-        <v>80.95</v>
+        <v>80.97</v>
       </c>
       <c r="C83" s="2">
-        <v>78.44</v>
+        <v>78.42</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1427,10 +1428,10 @@
         <v>43686</v>
       </c>
       <c r="B84" s="2">
-        <v>82.69</v>
+        <v>82.78</v>
       </c>
       <c r="C84" s="2">
-        <v>82.04</v>
+        <v>82.06</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1438,10 +1439,10 @@
         <v>43693</v>
       </c>
       <c r="B85" s="2">
-        <v>81.069999999999993</v>
+        <v>81.05</v>
       </c>
       <c r="C85" s="2">
-        <v>82.25</v>
+        <v>82.26</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1449,10 +1450,10 @@
         <v>43700</v>
       </c>
       <c r="B86" s="2">
-        <v>81.180000000000007</v>
+        <v>81.19</v>
       </c>
       <c r="C86" s="2">
-        <v>82.07</v>
+        <v>82.06</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1460,10 +1461,10 @@
         <v>43707</v>
       </c>
       <c r="B87" s="2">
-        <v>80.260000000000005</v>
+        <v>80.239999999999995</v>
       </c>
       <c r="C87" s="2">
-        <v>81.599999999999994</v>
+        <v>81.58</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1471,10 +1472,10 @@
         <v>43714</v>
       </c>
       <c r="B88" s="2">
-        <v>80.84</v>
+        <v>80.86</v>
       </c>
       <c r="C88" s="2">
-        <v>82.95</v>
+        <v>82.97</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1482,10 +1483,10 @@
         <v>43720</v>
       </c>
       <c r="B89" s="2">
-        <v>80.84</v>
+        <v>80.86</v>
       </c>
       <c r="C89" s="2">
-        <v>83.15</v>
+        <v>83.16</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1493,7 +1494,7 @@
         <v>43728</v>
       </c>
       <c r="B90" s="2">
-        <v>81.180000000000007</v>
+        <v>81.2</v>
       </c>
       <c r="C90" s="2">
         <v>83.06</v>
@@ -1504,10 +1505,10 @@
         <v>43735</v>
       </c>
       <c r="B91" s="2">
-        <v>70.849999999999994</v>
+        <v>70.83</v>
       </c>
       <c r="C91" s="2">
-        <v>79.319999999999993</v>
+        <v>79.3</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1515,10 +1516,10 @@
         <v>43742</v>
       </c>
       <c r="B92" s="2">
-        <v>68.52</v>
+        <v>68.5</v>
       </c>
       <c r="C92" s="2">
-        <v>70.33</v>
+        <v>70.31</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1526,10 +1527,10 @@
         <v>43749</v>
       </c>
       <c r="B93" s="2">
-        <v>77</v>
+        <v>77.02</v>
       </c>
       <c r="C93" s="2">
-        <v>76.94</v>
+        <v>76.959999999999994</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1537,10 +1538,10 @@
         <v>43756</v>
       </c>
       <c r="B94" s="2">
-        <v>76.540000000000006</v>
+        <v>76.52</v>
       </c>
       <c r="C94" s="2">
-        <v>78.010000000000005</v>
+        <v>78.03</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1548,10 +1549,10 @@
         <v>43763</v>
       </c>
       <c r="B95" s="2">
-        <v>76.77</v>
+        <v>76.78</v>
       </c>
       <c r="C95" s="2">
-        <v>77.239999999999995</v>
+        <v>77.22</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1559,10 +1560,10 @@
         <v>43770</v>
       </c>
       <c r="B96" s="2">
-        <v>77.930000000000007</v>
+        <v>77.95</v>
       </c>
       <c r="C96" s="2">
-        <v>78.48</v>
+        <v>78.540000000000006</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1570,10 +1571,10 @@
         <v>43777</v>
       </c>
       <c r="B97" s="2">
-        <v>76.540000000000006</v>
+        <v>76.52</v>
       </c>
       <c r="C97" s="2">
-        <v>77.39</v>
+        <v>77.37</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1581,10 +1582,10 @@
         <v>43784</v>
       </c>
       <c r="B98" s="2">
-        <v>77.930000000000007</v>
+        <v>77.95</v>
       </c>
       <c r="C98" s="2">
-        <v>78.760000000000005</v>
+        <v>78.78</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1592,10 +1593,10 @@
         <v>43791</v>
       </c>
       <c r="B99" s="2">
-        <v>77.239999999999995</v>
+        <v>77.22</v>
       </c>
       <c r="C99" s="2">
-        <v>78.47</v>
+        <v>78.459999999999994</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1603,10 +1604,10 @@
         <v>43798</v>
       </c>
       <c r="B100" s="2">
-        <v>78.28</v>
+        <v>78.3</v>
       </c>
       <c r="C100" s="2">
-        <v>79.89</v>
+        <v>79.91</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1614,10 +1615,10 @@
         <v>43805</v>
       </c>
       <c r="B101" s="2">
-        <v>79.09</v>
+        <v>79.11</v>
       </c>
       <c r="C101" s="2">
-        <v>80.94</v>
+        <v>80.959999999999994</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1625,10 +1626,10 @@
         <v>43812</v>
       </c>
       <c r="B102" s="2">
-        <v>77.819999999999993</v>
+        <v>77.760000000000005</v>
       </c>
       <c r="C102" s="2">
-        <v>80.23</v>
+        <v>80.209999999999994</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1636,10 +1637,10 @@
         <v>43819</v>
       </c>
       <c r="B103" s="2">
-        <v>77.819999999999993</v>
+        <v>77.760000000000005</v>
       </c>
       <c r="C103" s="2">
-        <v>79.23</v>
+        <v>79.209999999999994</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1647,10 +1648,10 @@
         <v>43826</v>
       </c>
       <c r="B104" s="2">
-        <v>76.89</v>
+        <v>76.87</v>
       </c>
       <c r="C104" s="2">
-        <v>78.989999999999995</v>
+        <v>78.98</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1658,10 +1659,10 @@
         <v>43833</v>
       </c>
       <c r="B105" s="2">
-        <v>78.400000000000006</v>
+        <v>78.42</v>
       </c>
       <c r="C105" s="2">
-        <v>79.650000000000006</v>
+        <v>79.67</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1669,10 +1670,10 @@
         <v>43840</v>
       </c>
       <c r="B106" s="2">
-        <v>77.58</v>
+        <v>77.56</v>
       </c>
       <c r="C106" s="2">
-        <v>79.41</v>
+        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1680,10 +1681,10 @@
         <v>43847</v>
       </c>
       <c r="B107" s="2">
-        <v>77.58</v>
+        <v>77.56</v>
       </c>
       <c r="C107" s="2">
-        <v>78.88</v>
+        <v>78.86</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1691,10 +1692,10 @@
         <v>43853</v>
       </c>
       <c r="B108" s="2">
-        <v>78.510000000000005</v>
+        <v>78.53</v>
       </c>
       <c r="C108" s="2">
-        <v>80.010000000000005</v>
+        <v>80.03</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1702,10 +1703,10 @@
         <v>43868</v>
       </c>
       <c r="B109" s="2">
-        <v>74.91</v>
+        <v>74.89</v>
       </c>
       <c r="C109" s="2">
-        <v>77.760000000000005</v>
+        <v>77.739999999999995</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1713,10 +1714,10 @@
         <v>43875</v>
       </c>
       <c r="B110" s="2">
-        <v>72.94</v>
+        <v>72.92</v>
       </c>
       <c r="C110" s="2">
-        <v>74.7</v>
+        <v>74.680000000000007</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1724,10 +1725,10 @@
         <v>43882</v>
       </c>
       <c r="B111" s="2">
-        <v>71.430000000000007</v>
+        <v>71.41</v>
       </c>
       <c r="C111" s="2">
-        <v>73.930000000000007</v>
+        <v>73.91</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1735,10 +1736,10 @@
         <v>43889</v>
       </c>
       <c r="B112" s="2">
-        <v>71.89</v>
+        <v>71.91</v>
       </c>
       <c r="C112" s="2">
-        <v>73.819999999999993</v>
+        <v>73.81</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1746,7 +1747,7 @@
         <v>43896</v>
       </c>
       <c r="B113" s="2">
-        <v>72.239999999999995</v>
+        <v>72.260000000000005</v>
       </c>
       <c r="C113" s="2">
         <v>73.78</v>
@@ -1757,10 +1758,10 @@
         <v>43903</v>
       </c>
       <c r="B114" s="2">
-        <v>72.59</v>
+        <v>72.61</v>
       </c>
       <c r="C114" s="2">
-        <v>73.900000000000006</v>
+        <v>73.91</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1768,10 +1769,10 @@
         <v>43910</v>
       </c>
       <c r="B115" s="2">
-        <v>73.75</v>
+        <v>73.77</v>
       </c>
       <c r="C115" s="2">
-        <v>75.260000000000005</v>
+        <v>75.28</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1779,10 +1780,10 @@
         <v>43917</v>
       </c>
       <c r="B116" s="2">
-        <v>75.260000000000005</v>
+        <v>75.28</v>
       </c>
       <c r="C116" s="2">
-        <v>76.19</v>
+        <v>76.209999999999994</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1790,10 +1791,10 @@
         <v>43924</v>
       </c>
       <c r="B117" s="2">
-        <v>77.349999999999994</v>
+        <v>77.37</v>
       </c>
       <c r="C117" s="2">
-        <v>77.8</v>
+        <v>77.819999999999993</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1801,10 +1802,10 @@
         <v>43931</v>
       </c>
       <c r="B118" s="2">
-        <v>78.86</v>
+        <v>78.88</v>
       </c>
       <c r="C118" s="2">
-        <v>78.81</v>
+        <v>78.83</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1812,10 +1813,10 @@
         <v>43938</v>
       </c>
       <c r="B119" s="2">
-        <v>80.489999999999995</v>
+        <v>80.510000000000005</v>
       </c>
       <c r="C119" s="2">
-        <v>79.97</v>
+        <v>80.03</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1823,10 +1824,10 @@
         <v>43945</v>
       </c>
       <c r="B120" s="2">
-        <v>80.489999999999995</v>
+        <v>80.510000000000005</v>
       </c>
       <c r="C120" s="2">
-        <v>80.59</v>
+        <v>80.61</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1834,10 +1835,10 @@
         <v>43951</v>
       </c>
       <c r="B121" s="2">
-        <v>80.95</v>
+        <v>80.97</v>
       </c>
       <c r="C121" s="2">
-        <v>81.680000000000007</v>
+        <v>81.7</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1845,10 +1846,10 @@
         <v>43959</v>
       </c>
       <c r="B122" s="2">
-        <v>88.28</v>
+        <v>88.3</v>
       </c>
       <c r="C122" s="2">
-        <v>89.1</v>
+        <v>89.12</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1856,10 +1857,10 @@
         <v>43966</v>
       </c>
       <c r="B123" s="2">
-        <v>89.84</v>
+        <v>89.86</v>
       </c>
       <c r="C123" s="2">
-        <v>89.94</v>
+        <v>89.98</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1867,10 +1868,10 @@
         <v>43973</v>
       </c>
       <c r="B124" s="2">
-        <v>90.49</v>
+        <v>90.51</v>
       </c>
       <c r="C124" s="2">
-        <v>90.95</v>
+        <v>90.97</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1878,10 +1879,10 @@
         <v>43980</v>
       </c>
       <c r="B125" s="2">
-        <v>91.02</v>
+        <v>91.05</v>
       </c>
       <c r="C125" s="2">
-        <v>91.38</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1889,10 +1890,10 @@
         <v>43987</v>
       </c>
       <c r="B126" s="2">
-        <v>91.02</v>
+        <v>91.05</v>
       </c>
       <c r="C126" s="2">
-        <v>91.9</v>
+        <v>91.93</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1900,10 +1901,10 @@
         <v>43994</v>
       </c>
       <c r="B127" s="2">
-        <v>91.67</v>
+        <v>91.69</v>
       </c>
       <c r="C127" s="2">
-        <v>92.35</v>
+        <v>92.37</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1911,10 +1912,10 @@
         <v>44001</v>
       </c>
       <c r="B128" s="2">
-        <v>91.54</v>
+        <v>91.53</v>
       </c>
       <c r="C128" s="2">
-        <v>92.66</v>
+        <v>92.68</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1922,10 +1923,10 @@
         <v>44008</v>
       </c>
       <c r="B129" s="2">
-        <v>91.8</v>
+        <v>91.81</v>
       </c>
       <c r="C129" s="2">
-        <v>93.42</v>
+        <v>93.44</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1933,7 +1934,7 @@
         <v>44015</v>
       </c>
       <c r="B130" s="2">
-        <v>91.02</v>
+        <v>91</v>
       </c>
       <c r="C130" s="2">
         <v>93.35</v>
@@ -1944,10 +1945,10 @@
         <v>44022</v>
       </c>
       <c r="B131" s="2">
-        <v>90.63</v>
+        <v>90.61</v>
       </c>
       <c r="C131" s="2">
-        <v>93.08</v>
+        <v>93.07</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1955,10 +1956,10 @@
         <v>44029</v>
       </c>
       <c r="B132" s="2">
-        <v>90.76</v>
+        <v>90.77</v>
       </c>
       <c r="C132" s="2">
-        <v>92.96</v>
+        <v>92.95</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1966,10 +1967,10 @@
         <v>44036</v>
       </c>
       <c r="B133" s="2">
-        <v>91.02</v>
+        <v>91.03</v>
       </c>
       <c r="C133" s="2">
-        <v>93.08</v>
+        <v>93.09</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1977,10 +1978,10 @@
         <v>44043</v>
       </c>
       <c r="B134" s="2">
-        <v>91.15</v>
+        <v>91.16</v>
       </c>
       <c r="C134" s="2">
-        <v>94.5</v>
+        <v>94.52</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1988,10 +1989,10 @@
         <v>44050</v>
       </c>
       <c r="B135" s="2">
-        <v>91.41</v>
+        <v>91.42</v>
       </c>
       <c r="C135" s="2">
-        <v>94.75</v>
+        <v>94.76</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1999,10 +2000,10 @@
         <v>44057</v>
       </c>
       <c r="B136" s="2">
-        <v>91.93</v>
+        <v>91.95</v>
       </c>
       <c r="C136" s="2">
-        <v>95.16</v>
+        <v>95.18</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2010,10 +2011,10 @@
         <v>44064</v>
       </c>
       <c r="B137" s="2">
-        <v>91.41</v>
+        <v>91.39</v>
       </c>
       <c r="C137" s="2">
-        <v>94.8</v>
+        <v>94.78</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2021,10 +2022,10 @@
         <v>44071</v>
       </c>
       <c r="B138" s="2">
-        <v>91.41</v>
+        <v>91.39</v>
       </c>
       <c r="C138" s="2">
-        <v>94.64</v>
+        <v>94.63</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2032,10 +2033,10 @@
         <v>44078</v>
       </c>
       <c r="B139" s="2">
-        <v>91.41</v>
+        <v>91.39</v>
       </c>
       <c r="C139" s="2">
-        <v>94.52</v>
+        <v>94.51</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2043,10 +2044,10 @@
         <v>44085</v>
       </c>
       <c r="B140" s="2">
-        <v>90.89</v>
+        <v>90.87</v>
       </c>
       <c r="C140" s="2">
-        <v>94.31</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2054,7 +2055,7 @@
         <v>44092</v>
       </c>
       <c r="B141" s="2">
-        <v>90.63</v>
+        <v>90.62</v>
       </c>
       <c r="C141" s="2">
         <v>94.25</v>
@@ -2065,10 +2066,10 @@
         <v>44099</v>
       </c>
       <c r="B142" s="2">
-        <v>89.06</v>
+        <v>89.04</v>
       </c>
       <c r="C142" s="2">
-        <v>93.69</v>
+        <v>93.67</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2076,10 +2077,10 @@
         <v>44104</v>
       </c>
       <c r="B143" s="2">
-        <v>88.54</v>
+        <v>88.52</v>
       </c>
       <c r="C143" s="2">
-        <v>93.04</v>
+        <v>93.01</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2087,10 +2088,10 @@
         <v>44113</v>
       </c>
       <c r="B144" s="2">
-        <v>89.19</v>
+        <v>89.21</v>
       </c>
       <c r="C144" s="2">
-        <v>93.2</v>
+        <v>93.21</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2098,10 +2099,10 @@
         <v>44120</v>
       </c>
       <c r="B145" s="2">
-        <v>88.41</v>
+        <v>88.39</v>
       </c>
       <c r="C145" s="2">
-        <v>92.91</v>
+        <v>92.9</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2109,10 +2110,10 @@
         <v>44127</v>
       </c>
       <c r="B146" s="2">
-        <v>88.28</v>
+        <v>88.27</v>
       </c>
       <c r="C146" s="2">
-        <v>92.34</v>
+        <v>92.31</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2120,10 +2121,10 @@
         <v>44134</v>
       </c>
       <c r="B147" s="2">
-        <v>87.5</v>
+        <v>87.48</v>
       </c>
       <c r="C147" s="2">
-        <v>92.47</v>
+        <v>92.48</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2131,10 +2132,10 @@
         <v>44141</v>
       </c>
       <c r="B148" s="2">
-        <v>86.46</v>
+        <v>86.44</v>
       </c>
       <c r="C148" s="2">
-        <v>92.27</v>
+        <v>92.26</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2142,10 +2143,10 @@
         <v>44148</v>
       </c>
       <c r="B149" s="2">
-        <v>86.33</v>
+        <v>86.32</v>
       </c>
       <c r="C149" s="2">
-        <v>92.11</v>
+        <v>92.1</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2153,10 +2154,10 @@
         <v>44155</v>
       </c>
       <c r="B150" s="2">
-        <v>86.46</v>
+        <v>86.47</v>
       </c>
       <c r="C150" s="2">
-        <v>91.64</v>
+        <v>91.62</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2164,10 +2165,10 @@
         <v>44162</v>
       </c>
       <c r="B151" s="2">
-        <v>86.33</v>
+        <v>86.32</v>
       </c>
       <c r="C151" s="2">
-        <v>92.47</v>
+        <v>92.49</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2175,7 +2176,7 @@
         <v>44169</v>
       </c>
       <c r="B152" s="2">
-        <v>85.42</v>
+        <v>85.4</v>
       </c>
       <c r="C152" s="2">
         <v>92.4</v>
@@ -2186,10 +2187,10 @@
         <v>44176</v>
       </c>
       <c r="B153" s="2">
-        <v>84.77</v>
+        <v>84.75</v>
       </c>
       <c r="C153" s="2">
-        <v>91.47</v>
+        <v>91.42</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2197,10 +2198,10 @@
         <v>44183</v>
       </c>
       <c r="B154" s="2">
-        <v>85.29</v>
+        <v>85.31</v>
       </c>
       <c r="C154" s="2">
-        <v>91.68</v>
+        <v>91.69</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2208,10 +2209,10 @@
         <v>44190</v>
       </c>
       <c r="B155" s="2">
-        <v>85.55</v>
+        <v>85.56</v>
       </c>
       <c r="C155" s="2">
-        <v>91.87</v>
+        <v>91.88</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2219,10 +2220,10 @@
         <v>44196</v>
       </c>
       <c r="B156" s="2">
-        <v>86.07</v>
+        <v>86.1</v>
       </c>
       <c r="C156" s="2">
-        <v>92.08</v>
+        <v>92.09</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2230,10 +2231,10 @@
         <v>44204</v>
       </c>
       <c r="B157" s="2">
-        <v>85.29</v>
+        <v>85.27</v>
       </c>
       <c r="C157" s="2">
-        <v>91.77</v>
+        <v>91.75</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2241,10 +2242,10 @@
         <v>44211</v>
       </c>
       <c r="B158" s="2">
-        <v>84.24</v>
+        <v>84.22</v>
       </c>
       <c r="C158" s="2">
-        <v>91.24</v>
+        <v>91.22</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2252,10 +2253,10 @@
         <v>44218</v>
       </c>
       <c r="B159" s="2">
-        <v>83.2</v>
+        <v>83.18</v>
       </c>
       <c r="C159" s="2">
-        <v>91.12</v>
+        <v>91.11</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2263,10 +2264,10 @@
         <v>44225</v>
       </c>
       <c r="B160" s="2">
-        <v>82.03</v>
+        <v>82.01</v>
       </c>
       <c r="C160" s="2">
-        <v>90.53</v>
+        <v>90.51</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2274,10 +2275,10 @@
         <v>44232</v>
       </c>
       <c r="B161" s="2">
-        <v>83.2</v>
+        <v>83.22</v>
       </c>
       <c r="C161" s="2">
-        <v>90.94</v>
+        <v>90.96</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2285,10 +2286,10 @@
         <v>44246</v>
       </c>
       <c r="B162" s="2">
-        <v>83.98</v>
+        <v>84</v>
       </c>
       <c r="C162" s="2">
-        <v>92.19</v>
+        <v>92.21</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2296,7 +2297,7 @@
         <v>44253</v>
       </c>
       <c r="B163" s="2">
-        <v>83.85</v>
+        <v>83.84</v>
       </c>
       <c r="C163" s="2">
         <v>92.28</v>
@@ -2307,10 +2308,10 @@
         <v>44260</v>
       </c>
       <c r="B164" s="2">
-        <v>83.33</v>
+        <v>83.31</v>
       </c>
       <c r="C164" s="2">
-        <v>92.05</v>
+        <v>92.04</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2318,10 +2319,10 @@
         <v>44267</v>
       </c>
       <c r="B165" s="2">
-        <v>80.34</v>
+        <v>80.319999999999993</v>
       </c>
       <c r="C165" s="2">
-        <v>90.39</v>
+        <v>90.37</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2329,10 +2330,10 @@
         <v>44274</v>
       </c>
       <c r="B166" s="2">
-        <v>79.69</v>
+        <v>79.67</v>
       </c>
       <c r="C166" s="2">
-        <v>87.16</v>
+        <v>87.14</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2340,10 +2341,10 @@
         <v>44281</v>
       </c>
       <c r="B167" s="2">
-        <v>79.56</v>
+        <v>79.55</v>
       </c>
       <c r="C167" s="2">
-        <v>88.3</v>
+        <v>88.32</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2351,10 +2352,10 @@
         <v>44288</v>
       </c>
       <c r="B168" s="2">
-        <v>77.47</v>
+        <v>77.37</v>
       </c>
       <c r="C168" s="2">
-        <v>86.92</v>
+        <v>86.9</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2362,7 +2363,7 @@
         <v>44295</v>
       </c>
       <c r="B169" s="2">
-        <v>77.86</v>
+        <v>77.88</v>
       </c>
       <c r="C169" s="2">
         <v>86.94</v>
@@ -2373,10 +2374,10 @@
         <v>44302</v>
       </c>
       <c r="B170" s="2">
-        <v>78.13</v>
+        <v>78.14</v>
       </c>
       <c r="C170" s="2">
-        <v>87.67</v>
+        <v>87.69</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2384,10 +2385,10 @@
         <v>44309</v>
       </c>
       <c r="B171" s="2">
-        <v>79.430000000000007</v>
+        <v>79.45</v>
       </c>
       <c r="C171" s="2">
-        <v>88.75</v>
+        <v>88.77</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2395,10 +2396,10 @@
         <v>44316</v>
       </c>
       <c r="B172" s="2">
-        <v>80.08</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="C172" s="2">
-        <v>89.93</v>
+        <v>89.95</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2406,10 +2407,10 @@
         <v>44323</v>
       </c>
       <c r="B173" s="2">
-        <v>80.47</v>
+        <v>80.489999999999995</v>
       </c>
       <c r="C173" s="2">
-        <v>90.59</v>
+        <v>90.61</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2417,10 +2418,10 @@
         <v>44330</v>
       </c>
       <c r="B174" s="2">
-        <v>80.34</v>
+        <v>80.33</v>
       </c>
       <c r="C174" s="2">
-        <v>90.87</v>
+        <v>90.88</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2428,10 +2429,10 @@
         <v>44337</v>
       </c>
       <c r="B175" s="2">
-        <v>80.209999999999994</v>
+        <v>80.2</v>
       </c>
       <c r="C175" s="2">
-        <v>91.18</v>
+        <v>91.2</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2439,10 +2440,10 @@
         <v>44344</v>
       </c>
       <c r="B176" s="2">
-        <v>80.989999999999995</v>
+        <v>81.010000000000005</v>
       </c>
       <c r="C176" s="2">
-        <v>91.41</v>
+        <v>91.42</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2450,10 +2451,10 @@
         <v>44351</v>
       </c>
       <c r="B177" s="2">
-        <v>80.86</v>
+        <v>80.849999999999994</v>
       </c>
       <c r="C177" s="2">
-        <v>91.89</v>
+        <v>91.91</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2461,10 +2462,10 @@
         <v>44358</v>
       </c>
       <c r="B178" s="2">
-        <v>80.34</v>
+        <v>80.319999999999993</v>
       </c>
       <c r="C178" s="2">
-        <v>91.69</v>
+        <v>91.68</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2472,7 +2473,7 @@
         <v>44365</v>
       </c>
       <c r="B179" s="2">
-        <v>80.209999999999994</v>
+        <v>80.2</v>
       </c>
       <c r="C179" s="2">
         <v>91.67</v>
@@ -2483,10 +2484,10 @@
         <v>44372</v>
       </c>
       <c r="B180" s="2">
-        <v>79.69</v>
+        <v>79.67</v>
       </c>
       <c r="C180" s="2">
-        <v>91.17</v>
+        <v>91.15</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2494,10 +2495,10 @@
         <v>44379</v>
       </c>
       <c r="B181" s="2">
-        <v>57.94</v>
+        <v>57.93</v>
       </c>
       <c r="C181" s="2">
-        <v>81.010000000000005</v>
+        <v>80.989999999999995</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2505,10 +2506,10 @@
         <v>44386</v>
       </c>
       <c r="B182" s="2">
-        <v>78.260000000000005</v>
+        <v>78.28</v>
       </c>
       <c r="C182" s="2">
-        <v>86</v>
+        <v>86.02</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2516,10 +2517,10 @@
         <v>44393</v>
       </c>
       <c r="B183" s="2">
-        <v>76.69</v>
+        <v>76.67</v>
       </c>
       <c r="C183" s="2">
-        <v>88.55</v>
+        <v>88.57</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2527,10 +2528,10 @@
         <v>44400</v>
       </c>
       <c r="B184" s="2">
-        <v>75.650000000000006</v>
+        <v>75.63</v>
       </c>
       <c r="C184" s="2">
-        <v>88.04</v>
+        <v>88.02</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2538,10 +2539,10 @@
         <v>44407</v>
       </c>
       <c r="B185" s="2">
-        <v>74.349999999999994</v>
+        <v>74.33</v>
       </c>
       <c r="C185" s="2">
-        <v>86.83</v>
+        <v>86.81</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2549,10 +2550,10 @@
         <v>44414</v>
       </c>
       <c r="B186" s="2">
-        <v>74.61</v>
+        <v>74.62</v>
       </c>
       <c r="C186" s="2">
-        <v>85.73</v>
+        <v>85.71</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2560,10 +2561,10 @@
         <v>44421</v>
       </c>
       <c r="B187" s="2">
-        <v>75</v>
+        <v>75.02</v>
       </c>
       <c r="C187" s="2">
-        <v>85.89</v>
+        <v>85.9</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2571,10 +2572,10 @@
         <v>44428</v>
       </c>
       <c r="B188" s="2">
-        <v>73.569999999999993</v>
+        <v>73.55</v>
       </c>
       <c r="C188" s="2">
-        <v>85.47</v>
+        <v>85.45</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2582,10 +2583,10 @@
         <v>44435</v>
       </c>
       <c r="B189" s="2">
-        <v>74.22</v>
+        <v>74.239999999999995</v>
       </c>
       <c r="C189" s="2">
-        <v>85.3</v>
+        <v>85.29</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2593,10 +2594,10 @@
         <v>44449</v>
       </c>
       <c r="B190" s="2">
-        <v>73.569999999999993</v>
+        <v>73.55</v>
       </c>
       <c r="C190" s="2">
-        <v>84.77</v>
+        <v>84.75</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2604,10 +2605,10 @@
         <v>44456</v>
       </c>
       <c r="B191" s="2">
-        <v>71.88</v>
+        <v>71.86</v>
       </c>
       <c r="C191" s="2">
-        <v>83.74</v>
+        <v>83.69</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -2615,10 +2616,10 @@
         <v>44463</v>
       </c>
       <c r="B192" s="2">
-        <v>69.92</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="C192" s="2">
-        <v>82.06</v>
+        <v>82.04</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -2626,10 +2627,10 @@
         <v>44469</v>
       </c>
       <c r="B193" s="2">
-        <v>73.239999999999995</v>
+        <v>73.260000000000005</v>
       </c>
       <c r="C193" s="2">
-        <v>78.69</v>
+        <v>78.67</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -2637,10 +2638,10 @@
         <v>44477</v>
       </c>
       <c r="B194" s="2">
-        <v>77.52</v>
+        <v>77.540000000000006</v>
       </c>
       <c r="C194" s="2">
-        <v>79.94</v>
+        <v>79.959999999999994</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -2648,10 +2649,10 @@
         <v>44484</v>
       </c>
       <c r="B195" s="2">
-        <v>78.069999999999993</v>
+        <v>78.09</v>
       </c>
       <c r="C195" s="2">
-        <v>80.66</v>
+        <v>80.680000000000007</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -2659,10 +2660,10 @@
         <v>44491</v>
       </c>
       <c r="B196" s="2">
-        <v>76.55</v>
+        <v>76.47</v>
       </c>
       <c r="C196" s="2">
-        <v>80.05</v>
+        <v>80.03</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -2670,10 +2671,10 @@
         <v>44498</v>
       </c>
       <c r="B197" s="2">
-        <v>74.900000000000006</v>
+        <v>74.88</v>
       </c>
       <c r="C197" s="2">
-        <v>78.83</v>
+        <v>78.81</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -2681,10 +2682,10 @@
         <v>44505</v>
       </c>
       <c r="B198" s="2">
-        <v>70.900000000000006</v>
+        <v>70.88</v>
       </c>
       <c r="C198" s="2">
-        <v>76.430000000000007</v>
+        <v>76.31</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -2692,10 +2693,10 @@
         <v>44512</v>
       </c>
       <c r="B199" s="2">
-        <v>71.59</v>
+        <v>71.61</v>
       </c>
       <c r="C199" s="2">
-        <v>75.72</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -2703,10 +2704,10 @@
         <v>44519</v>
       </c>
       <c r="B200" s="2">
-        <v>70.34</v>
+        <v>70.319999999999993</v>
       </c>
       <c r="C200" s="2">
-        <v>75.349999999999994</v>
+        <v>75.33</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -2714,10 +2715,10 @@
         <v>44526</v>
       </c>
       <c r="B201" s="2">
-        <v>69.66</v>
+        <v>69.64</v>
       </c>
       <c r="C201" s="2">
-        <v>75.23</v>
+        <v>75.22</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -2725,10 +2726,10 @@
         <v>44533</v>
       </c>
       <c r="B202" s="2">
-        <v>69.790000000000006</v>
+        <v>69.8</v>
       </c>
       <c r="C202" s="2">
-        <v>74.8</v>
+        <v>74.78</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -2736,10 +2737,10 @@
         <v>44540</v>
       </c>
       <c r="B203" s="2">
-        <v>68.14</v>
+        <v>68.12</v>
       </c>
       <c r="C203" s="2">
-        <v>74.12</v>
+        <v>74.099999999999994</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -2747,10 +2748,10 @@
         <v>44547</v>
       </c>
       <c r="B204" s="2">
-        <v>68</v>
+        <v>67.989999999999995</v>
       </c>
       <c r="C204" s="2">
-        <v>74.28</v>
+        <v>74.290000000000006</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -2758,7 +2759,7 @@
         <v>44554</v>
       </c>
       <c r="B205" s="2">
-        <v>67.87</v>
+        <v>67.86</v>
       </c>
       <c r="C205" s="2">
         <v>74.33</v>
@@ -2769,10 +2770,10 @@
         <v>44561</v>
       </c>
       <c r="B206" s="2">
-        <v>70.040000000000006</v>
+        <v>70.14</v>
       </c>
       <c r="C206" s="2">
-        <v>75.790000000000006</v>
+        <v>75.81</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -2780,10 +2781,10 @@
         <v>44568</v>
       </c>
       <c r="B207" s="2">
-        <v>74.2</v>
+        <v>74.3</v>
       </c>
       <c r="C207" s="2">
-        <v>77.89</v>
+        <v>77.91</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -2791,10 +2792,10 @@
         <v>44575</v>
       </c>
       <c r="B208" s="2">
-        <v>75.77</v>
+        <v>75.790000000000006</v>
       </c>
       <c r="C208" s="2">
-        <v>79.89</v>
+        <v>79.91</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -2802,10 +2803,10 @@
         <v>44582</v>
       </c>
       <c r="B209" s="2">
-        <v>76.25</v>
+        <v>76.27</v>
       </c>
       <c r="C209" s="2">
-        <v>81.08</v>
+        <v>81.099999999999994</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -2813,10 +2814,10 @@
         <v>44589</v>
       </c>
       <c r="B210" s="2">
-        <v>74.86</v>
+        <v>74.84</v>
       </c>
       <c r="C210" s="2">
-        <v>81.510000000000005</v>
+        <v>81.53</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -2824,10 +2825,10 @@
         <v>44603</v>
       </c>
       <c r="B211" s="2">
-        <v>68.19</v>
+        <v>68.180000000000007</v>
       </c>
       <c r="C211" s="2">
-        <v>76.569999999999993</v>
+        <v>76.47</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -2835,10 +2836,10 @@
         <v>44610</v>
       </c>
       <c r="B212" s="2">
-        <v>69.58</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="C212" s="2">
-        <v>75.44</v>
+        <v>75.42</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -2846,10 +2847,10 @@
         <v>44617</v>
       </c>
       <c r="B213" s="2">
-        <v>73.44</v>
+        <v>73.63</v>
       </c>
       <c r="C213" s="2">
-        <v>77.61</v>
+        <v>77.63</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -2857,10 +2858,10 @@
         <v>44624</v>
       </c>
       <c r="B214" s="2">
-        <v>74.72</v>
+        <v>74.739999999999995</v>
       </c>
       <c r="C214" s="2">
-        <v>81.489999999999995</v>
+        <v>81.510000000000005</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -2868,10 +2869,10 @@
         <v>44631</v>
       </c>
       <c r="B215" s="2">
-        <v>70.849999999999994</v>
+        <v>70.83</v>
       </c>
       <c r="C215" s="2">
-        <v>79.78</v>
+        <v>79.760000000000005</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -2879,10 +2880,10 @@
         <v>44638</v>
       </c>
       <c r="B216" s="2">
-        <v>78.91</v>
+        <v>79.010000000000005</v>
       </c>
       <c r="C216" s="2">
-        <v>81.88</v>
+        <v>81.900000000000006</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -2890,10 +2891,10 @@
         <v>44645</v>
       </c>
       <c r="B217" s="2">
-        <v>78.209999999999994</v>
+        <v>78.19</v>
       </c>
       <c r="C217" s="2">
-        <v>85.43</v>
+        <v>85.45</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -2901,10 +2902,10 @@
         <v>44652</v>
       </c>
       <c r="B218" s="2">
-        <v>77.45</v>
+        <v>77.430000000000007</v>
       </c>
       <c r="C218" s="2">
-        <v>83.76</v>
+        <v>83.74</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -2912,10 +2913,10 @@
         <v>44659</v>
       </c>
       <c r="B219" s="2">
-        <v>79.27</v>
+        <v>79.290000000000006</v>
       </c>
       <c r="C219" s="2">
-        <v>84.95</v>
+        <v>84.97</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -2923,10 +2924,10 @@
         <v>44666</v>
       </c>
       <c r="B220" s="2">
-        <v>80.11</v>
+        <v>80.13</v>
       </c>
       <c r="C220" s="2">
-        <v>86.42</v>
+        <v>86.44</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -2934,7 +2935,7 @@
         <v>44673</v>
       </c>
       <c r="B221" s="2">
-        <v>79.8</v>
+        <v>79.78</v>
       </c>
       <c r="C221" s="2">
         <v>86.35</v>
@@ -2945,10 +2946,10 @@
         <v>44680</v>
       </c>
       <c r="B222" s="2">
-        <v>80.930000000000007</v>
+        <v>80.95</v>
       </c>
       <c r="C222" s="2">
-        <v>86.57</v>
+        <v>86.58</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -2956,10 +2957,10 @@
         <v>44687</v>
       </c>
       <c r="B223" s="2">
-        <v>81.91</v>
+        <v>81.93</v>
       </c>
       <c r="C223" s="2">
-        <v>87.75</v>
+        <v>87.77</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -2967,10 +2968,10 @@
         <v>44694</v>
       </c>
       <c r="B224" s="2">
-        <v>82.61</v>
+        <v>82.63</v>
       </c>
       <c r="C224" s="2">
-        <v>88.28</v>
+        <v>88.3</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -2978,10 +2979,10 @@
         <v>44701</v>
       </c>
       <c r="B225" s="2">
-        <v>83.01</v>
+        <v>83.03</v>
       </c>
       <c r="C225" s="2">
-        <v>88.66</v>
+        <v>88.68</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -2989,10 +2990,10 @@
         <v>44708</v>
       </c>
       <c r="B226" s="2">
-        <v>83.83</v>
+        <v>83.85</v>
       </c>
       <c r="C226" s="2">
-        <v>89.26</v>
+        <v>89.28</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3000,10 +3001,10 @@
         <v>44714</v>
       </c>
       <c r="B227" s="2">
-        <v>83.68</v>
+        <v>83.67</v>
       </c>
       <c r="C227" s="2">
-        <v>89.9</v>
+        <v>89.92</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3011,10 +3012,10 @@
         <v>44722</v>
       </c>
       <c r="B228" s="2">
-        <v>84.11</v>
+        <v>84.13</v>
       </c>
       <c r="C228" s="2">
-        <v>90.14</v>
+        <v>90.15</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3022,7 +3023,7 @@
         <v>44729</v>
       </c>
       <c r="B229" s="2">
-        <v>83.83</v>
+        <v>83.82</v>
       </c>
       <c r="C229" s="2">
         <v>90.15</v>
@@ -3033,10 +3034,10 @@
         <v>44736</v>
       </c>
       <c r="B230" s="2">
-        <v>81.92</v>
+        <v>81.819999999999993</v>
       </c>
       <c r="C230" s="2">
-        <v>88.98</v>
+        <v>88.96</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3044,10 +3045,10 @@
         <v>44743</v>
       </c>
       <c r="B231" s="2">
-        <v>80.790000000000006</v>
+        <v>80.77</v>
       </c>
       <c r="C231" s="2">
-        <v>87.61</v>
+        <v>87.59</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3055,10 +3056,10 @@
         <v>44750</v>
       </c>
       <c r="B232" s="2">
-        <v>78.53</v>
+        <v>78.510000000000005</v>
       </c>
       <c r="C232" s="2">
-        <v>85.71</v>
+        <v>85.69</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3066,10 +3067,10 @@
         <v>44757</v>
       </c>
       <c r="B233" s="2">
-        <v>76.98</v>
+        <v>76.959999999999994</v>
       </c>
       <c r="C233" s="2">
-        <v>84.01</v>
+        <v>83.99</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3077,10 +3078,10 @@
         <v>44764</v>
       </c>
       <c r="B234" s="2">
-        <v>73.16</v>
+        <v>73.14</v>
       </c>
       <c r="C234" s="2">
-        <v>81.400000000000006</v>
+        <v>81.38</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3088,10 +3089,10 @@
         <v>44771</v>
       </c>
       <c r="B235" s="2">
-        <v>71.61</v>
+        <v>71.59</v>
       </c>
       <c r="C235" s="2">
-        <v>79.3</v>
+        <v>79.28</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3099,10 +3100,10 @@
         <v>44778</v>
       </c>
       <c r="B236" s="2">
-        <v>72.7</v>
+        <v>72.72</v>
       </c>
       <c r="C236" s="2">
-        <v>79.599999999999994</v>
+        <v>79.62</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3110,10 +3111,10 @@
         <v>44785</v>
       </c>
       <c r="B237" s="2">
-        <v>76.239999999999995</v>
+        <v>76.260000000000005</v>
       </c>
       <c r="C237" s="2">
-        <v>81.22</v>
+        <v>81.239999999999995</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3121,10 +3122,10 @@
         <v>44792</v>
       </c>
       <c r="B238" s="2">
-        <v>77.900000000000006</v>
+        <v>77.92</v>
       </c>
       <c r="C238" s="2">
-        <v>83.89</v>
+        <v>83.91</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3132,10 +3133,10 @@
         <v>44799</v>
       </c>
       <c r="B239" s="2">
-        <v>80.14</v>
+        <v>80.16</v>
       </c>
       <c r="C239" s="2">
-        <v>85.27</v>
+        <v>85.29</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3143,10 +3144,10 @@
         <v>44806</v>
       </c>
       <c r="B240" s="2">
-        <v>80.849999999999994</v>
+        <v>80.87</v>
       </c>
       <c r="C240" s="2">
-        <v>86.83</v>
+        <v>86.85</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3154,10 +3155,10 @@
         <v>44813</v>
       </c>
       <c r="B241" s="2">
-        <v>81.99</v>
+        <v>82.01</v>
       </c>
       <c r="C241" s="2">
-        <v>87.56</v>
+        <v>87.58</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3165,10 +3166,10 @@
         <v>44820</v>
       </c>
       <c r="B242" s="2">
-        <v>82.41</v>
+        <v>82.43</v>
       </c>
       <c r="C242" s="2">
-        <v>88.32</v>
+        <v>88.35</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3176,10 +3177,10 @@
         <v>44827</v>
       </c>
       <c r="B243" s="2">
-        <v>82.81</v>
+        <v>82.83</v>
       </c>
       <c r="C243" s="2">
-        <v>89.08</v>
+        <v>89.12</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3187,7 +3188,7 @@
         <v>44834</v>
       </c>
       <c r="B244" s="2">
-        <v>82.81</v>
+        <v>82.83</v>
       </c>
       <c r="C244" s="2">
         <v>89.14</v>
@@ -3198,10 +3199,10 @@
         <v>44842</v>
       </c>
       <c r="B245" s="2">
-        <v>83.5</v>
+        <v>83.53</v>
       </c>
       <c r="C245" s="2">
-        <v>88.98</v>
+        <v>88.97</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3209,7 +3210,7 @@
         <v>44848</v>
       </c>
       <c r="B246" s="2">
-        <v>82.62</v>
+        <v>82.6</v>
       </c>
       <c r="C246" s="2">
         <v>89.04</v>
@@ -3220,10 +3221,10 @@
         <v>44855</v>
       </c>
       <c r="B247" s="2">
-        <v>82.05</v>
+        <v>82.02</v>
       </c>
       <c r="C247" s="2">
-        <v>88.26</v>
+        <v>88.24</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3231,10 +3232,10 @@
         <v>44862</v>
       </c>
       <c r="B248" s="2">
-        <v>81.48</v>
+        <v>81.459999999999994</v>
       </c>
       <c r="C248" s="2">
-        <v>87.64</v>
+        <v>87.62</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3242,10 +3243,10 @@
         <v>44869</v>
       </c>
       <c r="B249" s="2">
-        <v>78.77</v>
+        <v>78.75</v>
       </c>
       <c r="C249" s="2">
-        <v>86.31</v>
+        <v>86.29</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3253,10 +3254,10 @@
         <v>44876</v>
       </c>
       <c r="B250" s="2">
-        <v>77.209999999999994</v>
+        <v>77.19</v>
       </c>
       <c r="C250" s="2">
-        <v>84.09</v>
+        <v>84.07</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3264,10 +3265,10 @@
         <v>44883</v>
       </c>
       <c r="B251" s="2">
-        <v>76.349999999999994</v>
+        <v>76.33</v>
       </c>
       <c r="C251" s="2">
-        <v>83.36</v>
+        <v>83.34</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3275,10 +3276,10 @@
         <v>44890</v>
       </c>
       <c r="B252" s="2">
-        <v>77.03</v>
+        <v>77.05</v>
       </c>
       <c r="C252" s="2">
-        <v>82.52</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3286,10 +3287,10 @@
         <v>44897</v>
       </c>
       <c r="B253" s="2">
-        <v>75.61</v>
+        <v>75.59</v>
       </c>
       <c r="C253" s="2">
-        <v>82.62</v>
+        <v>82.63</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3297,10 +3298,10 @@
         <v>44904</v>
       </c>
       <c r="B254" s="2">
-        <v>75.89</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="C254" s="2">
-        <v>82</v>
+        <v>81.98</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -3311,7 +3312,7 @@
         <v>75.97</v>
       </c>
       <c r="C255" s="2">
-        <v>82.64</v>
+        <v>82.66</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -3322,7 +3323,7 @@
         <v>75.930000000000007</v>
       </c>
       <c r="C256" s="2">
-        <v>82.39</v>
+        <v>82.38</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -3330,10 +3331,10 @@
         <v>44925</v>
       </c>
       <c r="B257" s="2">
-        <v>75.209999999999994</v>
+        <v>75.19</v>
       </c>
       <c r="C257" s="2">
-        <v>82.59</v>
+        <v>82.6</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -3341,10 +3342,10 @@
         <v>44932</v>
       </c>
       <c r="B258" s="2">
-        <v>74.64</v>
+        <v>74.62</v>
       </c>
       <c r="C258" s="2">
-        <v>81.93</v>
+        <v>81.91</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -3352,10 +3353,10 @@
         <v>44939</v>
       </c>
       <c r="B259" s="2">
-        <v>75.680000000000007</v>
+        <v>75.7</v>
       </c>
       <c r="C259" s="2">
-        <v>82.56</v>
+        <v>82.58</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -3363,10 +3364,10 @@
         <v>44946</v>
       </c>
       <c r="B260" s="2">
-        <v>75.97</v>
+        <v>75.98</v>
       </c>
       <c r="C260" s="2">
-        <v>83.1</v>
+        <v>83.12</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -3374,10 +3375,10 @@
         <v>44953</v>
       </c>
       <c r="B261" s="2">
-        <v>76.69</v>
+        <v>76.709999999999994</v>
       </c>
       <c r="C261" s="2">
-        <v>84.15</v>
+        <v>84.17</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -3385,10 +3386,10 @@
         <v>44960</v>
       </c>
       <c r="B262" s="2">
-        <v>77.41</v>
+        <v>77.430000000000007</v>
       </c>
       <c r="C262" s="2">
-        <v>84.32</v>
+        <v>84.33</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -3396,10 +3397,10 @@
         <v>44967</v>
       </c>
       <c r="B263" s="2">
-        <v>78.42</v>
+        <v>78.44</v>
       </c>
       <c r="C263" s="2">
-        <v>84.93</v>
+        <v>84.96</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -3407,10 +3408,10 @@
         <v>44974</v>
       </c>
       <c r="B264" s="2">
-        <v>79.540000000000006</v>
+        <v>79.56</v>
       </c>
       <c r="C264" s="2">
-        <v>85.75</v>
+        <v>85.77</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -3418,10 +3419,10 @@
         <v>44981</v>
       </c>
       <c r="B265" s="2">
-        <v>80.98</v>
+        <v>81</v>
       </c>
       <c r="C265" s="2">
-        <v>86.97</v>
+        <v>86.99</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -3432,7 +3433,7 @@
         <v>81.069999999999993</v>
       </c>
       <c r="C266" s="2">
-        <v>87.15</v>
+        <v>87.16</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -3440,10 +3441,10 @@
         <v>44995</v>
       </c>
       <c r="B267" s="2">
-        <v>82</v>
+        <v>82.02</v>
       </c>
       <c r="C267" s="2">
-        <v>88.03</v>
+        <v>88.05</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -3451,10 +3452,10 @@
         <v>45002</v>
       </c>
       <c r="B268" s="2">
-        <v>82.29</v>
+        <v>82.3</v>
       </c>
       <c r="C268" s="2">
-        <v>88.44</v>
+        <v>88.46</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -3462,10 +3463,10 @@
         <v>45009</v>
       </c>
       <c r="B269" s="2">
-        <v>82.73</v>
+        <v>82.75</v>
       </c>
       <c r="C269" s="2">
-        <v>89.28</v>
+        <v>89.32</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -3473,10 +3474,10 @@
         <v>45016</v>
       </c>
       <c r="B270" s="2">
-        <v>83.87</v>
+        <v>83.89</v>
       </c>
       <c r="C270" s="2">
-        <v>90.56</v>
+        <v>90.58</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -3484,10 +3485,10 @@
         <v>45023</v>
       </c>
       <c r="B271" s="2">
-        <v>84.3</v>
+        <v>84.32</v>
       </c>
       <c r="C271" s="2">
-        <v>91.2</v>
+        <v>91.23</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -3495,10 +3496,10 @@
         <v>45030</v>
       </c>
       <c r="B272" s="2">
-        <v>84.74</v>
+        <v>84.76</v>
       </c>
       <c r="C272" s="2">
-        <v>91.8</v>
+        <v>91.83</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -3506,10 +3507,10 @@
         <v>45037</v>
       </c>
       <c r="B273" s="2">
-        <v>84.59</v>
+        <v>84.58</v>
       </c>
       <c r="C273" s="2">
-        <v>91.5</v>
+        <v>91.49</v>
       </c>
     </row>
     <row r="274" spans="1:3">
@@ -3517,10 +3518,10 @@
         <v>45044</v>
       </c>
       <c r="B274" s="2">
-        <v>82.56</v>
+        <v>82.54</v>
       </c>
       <c r="C274" s="2">
-        <v>90.63</v>
+        <v>90.61</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -3528,10 +3529,10 @@
         <v>45051</v>
       </c>
       <c r="B275" s="2">
-        <v>81.69</v>
+        <v>81.67</v>
       </c>
       <c r="C275" s="2">
-        <v>89.49</v>
+        <v>89.47</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -3539,10 +3540,10 @@
         <v>45058</v>
       </c>
       <c r="B276" s="2">
-        <v>81.099999999999994</v>
+        <v>81.069999999999993</v>
       </c>
       <c r="C276" s="2">
-        <v>89.03</v>
+        <v>89.01</v>
       </c>
     </row>
     <row r="277" spans="1:3">
@@ -3550,7 +3551,7 @@
         <v>45065</v>
       </c>
       <c r="B277" s="2">
-        <v>82.36</v>
+        <v>82.38</v>
       </c>
       <c r="C277" s="2">
         <v>89.12</v>
@@ -3561,10 +3562,10 @@
         <v>45072</v>
       </c>
       <c r="B278" s="2">
-        <v>82.36</v>
+        <v>82.38</v>
       </c>
       <c r="C278" s="2">
-        <v>89.93</v>
+        <v>89.95</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -3572,10 +3573,10 @@
         <v>45079</v>
       </c>
       <c r="B279" s="2">
-        <v>82.36</v>
+        <v>82.38</v>
       </c>
       <c r="C279" s="2">
-        <v>89.66</v>
+        <v>89.65</v>
       </c>
     </row>
     <row r="280" spans="1:3">
@@ -3583,7 +3584,7 @@
         <v>45086</v>
       </c>
       <c r="B280" s="2">
-        <v>82.36</v>
+        <v>82.38</v>
       </c>
       <c r="C280" s="2">
         <v>89.67</v>
@@ -3594,10 +3595,10 @@
         <v>45093</v>
       </c>
       <c r="B281" s="2">
-        <v>83.09</v>
+        <v>83.11</v>
       </c>
       <c r="C281" s="2">
-        <v>90.32</v>
+        <v>90.35</v>
       </c>
     </row>
     <row r="282" spans="1:3">
@@ -3605,10 +3606,10 @@
         <v>45100</v>
       </c>
       <c r="B282" s="2">
-        <v>84.09</v>
+        <v>84.11</v>
       </c>
       <c r="C282" s="2">
-        <v>91.6</v>
+        <v>91.66</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -3616,10 +3617,10 @@
         <v>45107</v>
       </c>
       <c r="B283" s="2">
-        <v>84.09</v>
+        <v>84.11</v>
       </c>
       <c r="C283" s="2">
-        <v>91.98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="284" spans="1:3">
@@ -3627,10 +3628,208 @@
         <v>45114</v>
       </c>
       <c r="B284" s="2">
-        <v>84.48</v>
+        <v>84.5</v>
       </c>
       <c r="C284" s="2">
-        <v>92.11</v>
+        <v>92.12</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" s="5">
+        <v>45121</v>
+      </c>
+      <c r="B285" s="2">
+        <v>84.32</v>
+      </c>
+      <c r="C285" s="2">
+        <v>91.18</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" s="5">
+        <v>45128</v>
+      </c>
+      <c r="B286" s="2">
+        <v>83.58</v>
+      </c>
+      <c r="C286" s="2">
+        <v>91.16</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" s="5">
+        <v>45135</v>
+      </c>
+      <c r="B287" s="2">
+        <v>82.12</v>
+      </c>
+      <c r="C287" s="2">
+        <v>89.79</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" s="5">
+        <v>45142</v>
+      </c>
+      <c r="B288" s="2">
+        <v>83.38</v>
+      </c>
+      <c r="C288" s="2">
+        <v>90.06</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" s="5">
+        <v>45149</v>
+      </c>
+      <c r="B289" s="2">
+        <v>83.82</v>
+      </c>
+      <c r="C289" s="2">
+        <v>91.06</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" s="5">
+        <v>45156</v>
+      </c>
+      <c r="B290" s="2">
+        <v>84.1</v>
+      </c>
+      <c r="C290" s="2">
+        <v>91.81</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" s="5">
+        <v>45163</v>
+      </c>
+      <c r="B291" s="2">
+        <v>83.34</v>
+      </c>
+      <c r="C291" s="2">
+        <v>91.77</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" s="5">
+        <v>45170</v>
+      </c>
+      <c r="B292" s="2">
+        <v>84.11</v>
+      </c>
+      <c r="C292" s="2">
+        <v>92.3</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" s="5">
+        <v>45177</v>
+      </c>
+      <c r="B293" s="2">
+        <v>84.41</v>
+      </c>
+      <c r="C293" s="2">
+        <v>92.78</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" s="5">
+        <v>45184</v>
+      </c>
+      <c r="B294" s="2">
+        <v>84.05</v>
+      </c>
+      <c r="C294" s="2">
+        <v>92.64</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" s="5">
+        <v>45191</v>
+      </c>
+      <c r="B295" s="2">
+        <v>84.47</v>
+      </c>
+      <c r="C295" s="2">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" s="5">
+        <v>45197</v>
+      </c>
+      <c r="B296" s="2">
+        <v>84.15</v>
+      </c>
+      <c r="C296" s="2">
+        <v>93.1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" s="5">
+        <v>45206</v>
+      </c>
+      <c r="B297" s="2">
+        <v>83.39</v>
+      </c>
+      <c r="C297" s="2">
+        <v>92.29</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" s="5">
+        <v>45212</v>
+      </c>
+      <c r="B298" s="2">
+        <v>82.18</v>
+      </c>
+      <c r="C298" s="2">
+        <v>91.9</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299" s="5">
+        <v>45219</v>
+      </c>
+      <c r="B299" s="2">
+        <v>82.36</v>
+      </c>
+      <c r="C299" s="2">
+        <v>90.6</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="A300" s="5">
+        <v>45226</v>
+      </c>
+      <c r="B300" s="2">
+        <v>82.51</v>
+      </c>
+      <c r="C300" s="2">
+        <v>90.75</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301" s="5">
+        <v>45233</v>
+      </c>
+      <c r="B301" s="2">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="C301" s="2">
+        <v>90.21</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" s="5">
+        <v>45240</v>
+      </c>
+      <c r="B302" s="2">
+        <v>81.03</v>
+      </c>
+      <c r="C302" s="2">
+        <v>89.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-update with latest from WIND
</commit_message>
<xml_diff>
--- a/inst/extdata/China_ Blast Furnace Starting Rate (247)_ Nationwide.xlsx
+++ b/inst/extdata/China_ Blast Furnace Starting Rate (247)_ Nationwide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wind\Desktop\automation\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CD6FAF-FA5A-40F9-A5CF-1FFDB1421413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78577800-B9B1-4C4A-A0B0-F661E2C19B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="11520" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,10 +101,10 @@
     <t>Wind</t>
   </si>
   <si>
-    <t>2018-03-02:2024-10-11</t>
+    <t>2018-03-02:2024-10-18</t>
   </si>
   <si>
-    <t>2024-10-11</t>
+    <t>2024-10-18</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C350"/>
+  <dimension ref="A1:C351"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E315" sqref="E315"/>
@@ -4362,6 +4362,17 @@
         <v>87.53</v>
       </c>
     </row>
+    <row r="351" spans="1:3">
+      <c r="A351" s="3">
+        <v>45583</v>
+      </c>
+      <c r="B351" s="2">
+        <v>81.7</v>
+      </c>
+      <c r="C351" s="2">
+        <v>88.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>